<commit_message>
[BE] template - fix user template
</commit_message>
<xml_diff>
--- a/packages/backend_php/public/templates/UserTemplate.xlsx
+++ b/packages/backend_php/public/templates/UserTemplate.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HOC-TAP\KLTN\source\packages\backend_php\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E254753-EFA3-44CD-879A-B04AFBB72AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039C727A-EFF0-4B48-8C6B-4C6DDE0FDEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="DATA" sheetId="3" r:id="rId1"/>
+    <sheet name="Gender" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -187,9 +187,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -470,21 +468,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4194EA-7831-40E8-A487-FA5D032E82DF}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="52" style="6" customWidth="1"/>
-    <col min="3" max="3" width="55.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="24.21875" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="15.88671875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="3" max="3" width="66.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -498,7 +495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -508,29 +505,23 @@
       <c r="C2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{DFDA9165-EC5F-4971-838D-FD4480541E1D}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{73FBB1FA-B6E3-4942-A8E9-933E8C376D1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{166B282E-282F-4A02-9E9B-B2BE6DAD77A0}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5E500379-917E-4229-8E87-A5CDD4115923}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$2:$A$3</xm:f>
+            <xm:f>Gender!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D2 D2:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>